<commit_message>
Quota Simulation Workload Generator > Update
</commit_message>
<xml_diff>
--- a/DMS-GridSim/workload/result/100000.xlsx
+++ b/DMS-GridSim/workload/result/100000.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="24">
   <si>
     <t>NP</t>
   </si>
@@ -73,6 +73,21 @@
   </si>
   <si>
     <t>EQ</t>
+  </si>
+  <si>
+    <t>TOTAL RUN TIME</t>
+  </si>
+  <si>
+    <t>Estático</t>
+  </si>
+  <si>
+    <t>Elástico</t>
+  </si>
+  <si>
+    <t>Elástica</t>
+  </si>
+  <si>
+    <t>Estática</t>
   </si>
 </sst>
 </file>
@@ -185,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -205,6 +220,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -317,11 +335,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="0"/>
-        <c:axId val="68357120"/>
-        <c:axId val="79869440"/>
+        <c:axId val="59725696"/>
+        <c:axId val="59732352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68357120"/>
+        <c:axId val="59725696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -360,14 +378,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79869440"/>
+        <c:crossAx val="59732352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79869440"/>
+        <c:axId val="59732352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -402,7 +420,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68357120"/>
+        <c:crossAx val="59725696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -411,7 +429,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000086" footer="0.31496062000000086"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -514,11 +532,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="0"/>
-        <c:axId val="79897728"/>
-        <c:axId val="79899648"/>
+        <c:axId val="59756544"/>
+        <c:axId val="59758464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79897728"/>
+        <c:axId val="59756544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -552,14 +570,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79899648"/>
+        <c:crossAx val="59758464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79899648"/>
+        <c:axId val="59758464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -593,7 +611,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79897728"/>
+        <c:crossAx val="59756544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -602,7 +620,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -705,11 +723,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="0"/>
-        <c:axId val="79907456"/>
-        <c:axId val="79930112"/>
+        <c:axId val="59926016"/>
+        <c:axId val="59927936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79907456"/>
+        <c:axId val="59926016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,14 +761,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79930112"/>
+        <c:crossAx val="59927936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79930112"/>
+        <c:axId val="59927936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -784,7 +802,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79907456"/>
+        <c:crossAx val="59926016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -793,7 +811,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -901,11 +919,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="0"/>
-        <c:axId val="81863040"/>
-        <c:axId val="81864960"/>
+        <c:axId val="59948032"/>
+        <c:axId val="59962496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81863040"/>
+        <c:axId val="59948032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,14 +957,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81864960"/>
+        <c:crossAx val="59962496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81864960"/>
+        <c:axId val="59962496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -980,7 +998,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81863040"/>
+        <c:crossAx val="59948032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -989,7 +1007,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1092,11 +1110,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="0"/>
-        <c:axId val="81893248"/>
-        <c:axId val="81895424"/>
+        <c:axId val="59990784"/>
+        <c:axId val="59992704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81893248"/>
+        <c:axId val="59990784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,14 +1153,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81895424"/>
+        <c:crossAx val="59992704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81895424"/>
+        <c:axId val="59992704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1176,7 +1194,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81893248"/>
+        <c:crossAx val="59990784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1185,7 +1203,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1458,11 +1476,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="82044032"/>
-        <c:axId val="82046336"/>
+        <c:axId val="60108800"/>
+        <c:axId val="60111104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82044032"/>
+        <c:axId val="60108800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1502,14 +1520,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82046336"/>
+        <c:crossAx val="60111104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82046336"/>
+        <c:axId val="60111104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1500"/>
@@ -1528,7 +1546,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82044032"/>
+        <c:crossAx val="60108800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000"/>
@@ -1551,7 +1569,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000058" footer="0.31496062000000058"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1560,6 +1578,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:style val="27"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1568,11 +1587,15 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="pt-BR"/>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR"/>
-              <a:t>Média do Tempo de Execução Total</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Média</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> do Tempo de Execução Total</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1581,77 +1604,38 @@
     </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Quota!$B$4</c:f>
+              <c:f>Quota!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NQ</c:v>
+                  <c:v>Estática</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Quota!$C$3:$G$3</c:f>
+              <c:f>Quota!$C$19:$E$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>2516</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>2974</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Quota!$C$4:$G$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                  <c:v>2568</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1661,260 +1645,261 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Quota!$B$5</c:f>
+              <c:f>Quota!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SQ</c:v>
+                  <c:v>Elástica</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Quota!$C$3:$G$3</c:f>
+              <c:f>Quota!$C$20:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>2516</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>2840</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Quota!$C$5:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>5942</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5305</c:v>
+                  <c:v>2469</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Quota!$B$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>EQ</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:headEnd type="none"/>
-              <a:tailEnd type="none" w="med" len="med"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="star"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="threePt" dir="t"/>
-              </a:scene3d>
-              <a:sp3d>
-                <a:bevelT/>
-              </a:sp3d>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Quota!$C$3:$G$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Quota!$C$6:$G$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>5944</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5895</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5788</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5583</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5294</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="82031360"/>
-        <c:axId val="82033664"/>
-      </c:lineChart>
+        <c:dLbls/>
+        <c:axId val="63132800"/>
+        <c:axId val="63134336"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="82031360"/>
+        <c:axId val="63132800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:minorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr lang="pt-BR"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-BR"/>
-                  <a:t>% de Reuso dos Dados</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="pt-BR"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="82033664"/>
+        <c:crossAx val="63134336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82033664"/>
+        <c:axId val="63134336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3000"/>
+          <c:min val="2300"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
+        <c:crossAx val="63132800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="29"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="pt-BR"/>
+              <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Média do Tempo de Espera</a:t>
+            </a:r>
           </a:p>
-        </c:txPr>
-        <c:crossAx val="82031360"/>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Quota!$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estática</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Quota!$C$22:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Quota!$C$23:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4528</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3895</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Quota!$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Elástica</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Quota!$C$22:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Quota!$C$24:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4528</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3730</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:axId val="60936576"/>
+        <c:axId val="60938496"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="60936576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="60938496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="60938496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="3000"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="60936576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr lang="pt-BR"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2115,19 +2100,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>190501</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2137,6 +2122,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2938,10 +2953,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G9"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3036,8 +3051,115 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
+    <row r="13" spans="2:7">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>2516</v>
+      </c>
+      <c r="D19">
+        <v>2974</v>
+      </c>
+      <c r="E19">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>2516</v>
+      </c>
+      <c r="D20">
+        <v>2840</v>
+      </c>
+      <c r="E20">
+        <v>2469</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23">
+        <v>4528</v>
+      </c>
+      <c r="D23">
+        <v>6250</v>
+      </c>
+      <c r="E23">
+        <v>3895</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>4528</v>
+      </c>
+      <c r="D24">
+        <v>6100</v>
+      </c>
+      <c r="E24">
+        <v>3730</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>